<commit_message>
made a circuit diagram of my project
</commit_message>
<xml_diff>
--- a/Solar panel load data.xlsx
+++ b/Solar panel load data.xlsx
@@ -1,41 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\Project 4th year\4th year project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BMcClennon\Desktop\4th year project\SolarPanelCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE19D697-A298-4AE7-A4D0-98B94123755E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CD227A6-2387-4523-9F28-67D11FFA270B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>current</t>
   </si>
@@ -48,11 +38,44 @@
   <si>
     <t>voltage diff</t>
   </si>
+  <si>
+    <t>device</t>
+  </si>
+  <si>
+    <t>kettle</t>
+  </si>
+  <si>
+    <t>heater 1</t>
+  </si>
+  <si>
+    <t>heater 2</t>
+  </si>
+  <si>
+    <t>resistance</t>
+  </si>
+  <si>
+    <t>light bulb 1(100w)</t>
+  </si>
+  <si>
+    <t>light bulb 2(100w)</t>
+  </si>
+  <si>
+    <t>light bulb 3 (60w)</t>
+  </si>
+  <si>
+    <t>resistor</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>total resitance</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,6 +164,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -413,6 +437,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -535,6 +560,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -615,6 +641,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -622,7 +649,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -705,6 +731,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -963,6 +990,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1081,6 +1109,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1161,6 +1190,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1168,6 +1198,476 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Power Output for vs load Resistance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.8919339740205294</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5866703288507229</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9701803791044012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4233837716014577</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4516933391849687</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.981005567451819</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100.51</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>117.78152999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.282520000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75.878399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.265920000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.401449</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.666015999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.81296</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BA4A-4353-98C3-CFA3D458F55B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="411412591"/>
+        <c:axId val="411413423"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="411412591"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Load Resistance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> (Ohms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411413423"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="411413423"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Power Output (Watt)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411412591"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1283,6 +1783,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2315,20 +2855,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2384,6 +3440,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>857249</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>26669</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2688,19 +3774,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F6B5DE-6EFD-4DA0-A811-5089F03C02A9}">
-  <dimension ref="B1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -2713,8 +3801,17 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>24.33</v>
       </c>
@@ -2726,119 +3823,199 @@
         <v>4.8410000000000002</v>
       </c>
       <c r="E2">
-        <f>B2*D2</f>
+        <f t="shared" ref="E2:E9" si="0">B2*D2</f>
         <v>117.78152999999999</v>
       </c>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>14.93</v>
+      </c>
+      <c r="P2">
+        <f>1/(1/$N$8+1/$N$7+1/$N$6+1/$N$5+1/$N$4+1/$N$3+1/$N$2)</f>
+        <v>2.8919339740205294</v>
+      </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>27.21</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C9" si="0">$B$9-B3</f>
+        <f t="shared" ref="C3:C9" si="1">$B$9-B3</f>
         <v>7.9159999999999968</v>
       </c>
       <c r="D3">
         <v>3.6120000000000001</v>
       </c>
       <c r="E3">
-        <f>B3*D3</f>
+        <f t="shared" si="0"/>
         <v>98.282520000000005</v>
       </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3">
+        <v>37.130000000000003</v>
+      </c>
+      <c r="O3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3">
+        <f>1/(1/$N$8+1/$N$7+1/$N$6+1/$N$5+1/$N$4+1/$N$3)</f>
+        <v>3.5866703288507229</v>
+      </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>29.64</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.4859999999999971</v>
       </c>
       <c r="D4">
         <v>2.56</v>
       </c>
       <c r="E4">
-        <f>B4*D4</f>
+        <f t="shared" si="0"/>
         <v>75.878399999999999</v>
       </c>
+      <c r="M4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4">
+        <v>38.75</v>
+      </c>
+      <c r="O4">
+        <f>AVERAGE(N3:N4)</f>
+        <v>37.94</v>
+      </c>
+      <c r="P4">
+        <f>1/(1/$N$8+1/$N$7+1/$N$6+1/$N$5+1/$N$4)</f>
+        <v>3.9701803791044012</v>
+      </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>32.287999999999997</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.838000000000001</v>
       </c>
       <c r="D5">
         <v>1.34</v>
       </c>
       <c r="E5">
-        <f>B5*D5</f>
+        <f t="shared" si="0"/>
         <v>43.265920000000001</v>
       </c>
+      <c r="M5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5">
+        <v>14.07</v>
+      </c>
+      <c r="P5">
+        <f>1/(1/$N$8+1/$N$7+1/$N$6+1/$N$5)</f>
+        <v>4.4233837716014577</v>
+      </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>33.029000000000003</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0969999999999942</v>
       </c>
       <c r="D6">
         <v>0.98099999999999998</v>
       </c>
       <c r="E6">
-        <f>B6*D6</f>
+        <f t="shared" si="0"/>
         <v>32.401449</v>
       </c>
+      <c r="M6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6">
+        <v>11.98</v>
+      </c>
+      <c r="P6">
+        <f>1/(1/$N$8+1/$N$7+1/$N$6)</f>
+        <v>6.4516933391849687</v>
+      </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>33.768000000000001</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.357999999999997</v>
       </c>
       <c r="D7">
         <v>0.61199999999999999</v>
       </c>
       <c r="E7">
-        <f>B7*D7</f>
+        <f t="shared" si="0"/>
         <v>20.666015999999999</v>
       </c>
+      <c r="M7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7">
+        <v>16.239999999999998</v>
+      </c>
+      <c r="P7">
+        <f>1/(1/$N$8+1/$N$7)</f>
+        <v>13.981005567451819</v>
+      </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>34.340000000000003</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.78599999999999426</v>
       </c>
       <c r="D8">
         <v>0.34399999999999997</v>
       </c>
       <c r="E8">
-        <f>B8*D8</f>
+        <f t="shared" si="0"/>
         <v>11.81296</v>
       </c>
+      <c r="M8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8">
+        <v>100.51</v>
+      </c>
+      <c r="P8">
+        <f>N8</f>
+        <v>100.51</v>
+      </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>35.125999999999998</v>
       </c>
       <c r="C9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <f>B9*D9</f>
+      <c r="P9">
         <v>0</v>
       </c>
     </row>

</xml_diff>